<commit_message>
formatting to word and latex actually works now
</commit_message>
<xml_diff>
--- a/hazards_dict.xlsx
+++ b/hazards_dict.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mauro\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\GitHub\GHSScraper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF8C9EE3-FDBE-4405-B1A2-AB215E1312EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{513CD3C3-6050-4603-A42F-BFFA6F9ADFA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-118" yWindow="-118" windowWidth="25370" windowHeight="13667" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="234">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="234">
   <si>
     <t>H200</t>
   </si>
@@ -777,17 +777,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1022,10 +1012,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:D112"/>
+  <dimension ref="A1:C112"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E107" sqref="E107"/>
+      <selection activeCell="D14" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1208,7 +1198,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>25</v>
       </c>
@@ -1219,7 +1209,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>27</v>
       </c>
@@ -1230,7 +1220,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>29</v>
       </c>
@@ -1241,7 +1231,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>31</v>
       </c>
@@ -1252,7 +1242,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>33</v>
       </c>
@@ -1261,7 +1251,7 @@
       </c>
       <c r="C21" s="2"/>
     </row>
-    <row r="22" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>35</v>
       </c>
@@ -1272,7 +1262,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="12.45" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" ht="12.45" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>37</v>
       </c>
@@ -1281,7 +1271,7 @@
       </c>
       <c r="C23" s="2"/>
     </row>
-    <row r="24" spans="1:4" ht="12.45" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" ht="12.45" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>39</v>
       </c>
@@ -1292,7 +1282,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="12.45" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" ht="12.45" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>41</v>
       </c>
@@ -1303,7 +1293,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="12.45" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3" ht="12.45" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>43</v>
       </c>
@@ -1314,7 +1304,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="12.45" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3" ht="12.45" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>45</v>
       </c>
@@ -1325,7 +1315,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="12.45" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3" ht="12.45" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>47</v>
       </c>
@@ -1335,11 +1325,8 @@
       <c r="C28" s="2" t="s">
         <v>223</v>
       </c>
-      <c r="D28" s="2" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" ht="12.45" x14ac:dyDescent="0.2">
+    </row>
+    <row r="29" spans="1:3" ht="12.45" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>49</v>
       </c>
@@ -1350,7 +1337,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="12.45" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3" ht="12.45" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>51</v>
       </c>
@@ -1361,7 +1348,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="12.45" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:3" ht="12.45" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>53</v>
       </c>
@@ -1372,7 +1359,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="12.45" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:3" ht="12.45" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>55</v>
       </c>
@@ -1383,7 +1370,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="12.45" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:3" ht="12.45" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>57</v>
       </c>
@@ -1394,7 +1381,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="12.45" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:3" ht="12.45" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>59</v>
       </c>
@@ -1405,7 +1392,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="12.45" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:3" ht="12.45" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>61</v>
       </c>
@@ -1416,7 +1403,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="12.45" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:3" ht="12.45" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>63</v>
       </c>
@@ -1427,7 +1414,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="12.45" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:3" ht="12.45" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>65</v>
       </c>
@@ -1438,7 +1425,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="12.45" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:3" ht="12.45" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>67</v>
       </c>
@@ -1449,7 +1436,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="12.45" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:3" ht="12.45" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>69</v>
       </c>
@@ -1459,11 +1446,8 @@
       <c r="C39" s="2" t="s">
         <v>226</v>
       </c>
-      <c r="D39" s="2" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" ht="12.45" x14ac:dyDescent="0.2">
+    </row>
+    <row r="40" spans="1:3" ht="12.45" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>71</v>
       </c>
@@ -1473,11 +1457,8 @@
       <c r="C40" s="2" t="s">
         <v>226</v>
       </c>
-      <c r="D40" s="2" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" ht="12.45" x14ac:dyDescent="0.2">
+    </row>
+    <row r="41" spans="1:3" ht="12.45" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>73</v>
       </c>
@@ -1488,7 +1469,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="12.45" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:3" ht="12.45" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>75</v>
       </c>
@@ -1499,7 +1480,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="12.45" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:3" ht="12.45" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>77</v>
       </c>
@@ -1510,7 +1491,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="12.45" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:3" ht="12.45" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>79</v>
       </c>
@@ -1521,7 +1502,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="45" spans="1:4" ht="12.45" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:3" ht="12.45" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
         <v>81</v>
       </c>
@@ -1532,7 +1513,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="46" spans="1:4" ht="12.45" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:3" ht="12.45" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
         <v>83</v>
       </c>
@@ -1543,7 +1524,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="47" spans="1:4" ht="12.45" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:3" ht="12.45" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
         <v>85</v>
       </c>
@@ -1551,7 +1532,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="48" spans="1:4" ht="12.45" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:3" ht="12.45" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
         <v>87</v>
       </c>

</xml_diff>

<commit_message>
final bugfixes, finished GUI
</commit_message>
<xml_diff>
--- a/hazards_dict.xlsx
+++ b/hazards_dict.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\GitHub\GHSScraper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{513CD3C3-6050-4603-A42F-BFFA6F9ADFA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A7160D3-F202-48AE-ACEF-4A6679256D49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-118" yWindow="-118" windowWidth="25370" windowHeight="13667" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="234">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="233">
   <si>
     <t>H200</t>
   </si>
@@ -713,9 +713,6 @@
   </si>
   <si>
     <t>health</t>
-  </si>
-  <si>
-    <t>excalm</t>
   </si>
   <si>
     <t>eclam</t>
@@ -1014,8 +1011,8 @@
   </sheetPr>
   <dimension ref="A1:C112"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D1:D1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="E58" sqref="E58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1614,7 +1611,7 @@
         <v>101</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="56" spans="1:3" ht="12.45" x14ac:dyDescent="0.2">
@@ -1633,7 +1630,7 @@
         <v>105</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="58" spans="1:3" ht="12.45" x14ac:dyDescent="0.2">
@@ -1967,7 +1964,7 @@
         <v>166</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="89" spans="1:3" ht="12.45" x14ac:dyDescent="0.2">
@@ -1994,7 +1991,7 @@
         <v>172</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="92" spans="1:3" ht="12.45" x14ac:dyDescent="0.2">
@@ -2005,7 +2002,7 @@
         <v>174</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="93" spans="1:3" ht="12.45" x14ac:dyDescent="0.2">

</xml_diff>